<commit_message>
fixed code response in step
</commit_message>
<xml_diff>
--- a/project-unit-tests/Test de regresion.xlsx
+++ b/project-unit-tests/Test de regresion.xlsx
@@ -53,13 +53,13 @@
     <t>1. Desde el browser hacer la peticion al servicio mediante wizdler extension para chrome
 2. Llamar al servicio http://localhost:54734/api/carriers/{id}
 3. Enviar el id del carrier que desea eliminar valor incorrecto
-4. El servidor responde statuscode=200 y un mensaje indicando si se pudo eliminar el registro</t>
+4. El servidor responde statuscode=400 y un mensaje indicando si se pudo eliminar el registro</t>
   </si>
   <si>
     <t>1. {id} ej 0</t>
   </si>
   <si>
-    <t>StatusCode = 200
+    <t>StatusCode = 400
 ErrorMessagesFromService[0].Description = "Carrier identifier is invalid"</t>
   </si>
   <si>

</xml_diff>